<commit_message>
Correct info on READ ME tabs
</commit_message>
<xml_diff>
--- a/Sample excel files/N_nineteen.xlsx
+++ b/Sample excel files/N_nineteen.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6948" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6948"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="7" r:id="rId1"/>
@@ -254,6 +254,72 @@
     <t xml:space="preserve">This can be done through the findit command in Stata. </t>
   </si>
   <si>
+    <t>This program has been made by BiostatGlobal Consulting and you may contact us with any questions. Contact information is listed below.</t>
+  </si>
+  <si>
+    <t>Dale Rhoda</t>
+  </si>
+  <si>
+    <t>Statistician &amp; President</t>
+  </si>
+  <si>
+    <t>Dale.Rhoda@biostatglobal.com</t>
+  </si>
+  <si>
+    <t>Mary Kay Trimner</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>MaryKay.Trimner@biostatglobal.com</t>
+  </si>
+  <si>
+    <t>ESS</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>gs7</t>
+  </si>
+  <si>
+    <t>Estimated Coverage %</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>foreground</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>Simple Random Sample: N=19</t>
+  </si>
+  <si>
+    <t>nineteen01, replace</t>
+  </si>
+  <si>
+    <t>nineteen01.png, width(2000) replace</t>
+  </si>
+  <si>
+    <t>80%</t>
+  </si>
+  <si>
+    <t>Text at right: point estimate; 1-sided tick marks at upper and lower 90% confidence bounds, size(vsmall) span</t>
+  </si>
+  <si>
+    <t>0 110</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Once the program has been downloaded you can use Stata help command to look up </t>
     </r>
@@ -267,7 +333,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>iwplot_vcqi</t>
+      <t>iwplot_svyp</t>
     </r>
     <r>
       <rPr>
@@ -301,72 +367,6 @@
       </rPr>
       <t>graph options for additional assistance.</t>
     </r>
-  </si>
-  <si>
-    <t>This program has been made by BiostatGlobal Consulting and you may contact us with any questions. Contact information is listed below.</t>
-  </si>
-  <si>
-    <t>Dale Rhoda</t>
-  </si>
-  <si>
-    <t>Statistician &amp; President</t>
-  </si>
-  <si>
-    <t>Dale.Rhoda@biostatglobal.com</t>
-  </si>
-  <si>
-    <t>Mary Kay Trimner</t>
-  </si>
-  <si>
-    <t>Project Manager</t>
-  </si>
-  <si>
-    <t>MaryKay.Trimner@biostatglobal.com</t>
-  </si>
-  <si>
-    <t>ESS</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>gs7</t>
-  </si>
-  <si>
-    <t>Estimated Coverage %</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>foreground</t>
-  </si>
-  <si>
-    <t>black</t>
-  </si>
-  <si>
-    <t>Wilson</t>
-  </si>
-  <si>
-    <t>Simple Random Sample: N=19</t>
-  </si>
-  <si>
-    <t>nineteen01, replace</t>
-  </si>
-  <si>
-    <t>nineteen01.png, width(2000) replace</t>
-  </si>
-  <si>
-    <t>80%</t>
-  </si>
-  <si>
-    <t>Text at right: point estimate; 1-sided tick marks at upper and lower 90% confidence bounds, size(vsmall) span</t>
-  </si>
-  <si>
-    <t>0 110</t>
   </si>
 </sst>
 </file>
@@ -974,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1082,7 +1082,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -1116,7 +1116,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -1150,16 +1150,16 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -1172,16 +1172,16 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" t="str">
         <f>_xlfn.CONCAT(ROUND(F2,1),"%")</f>
@@ -1477,13 +1477,13 @@
         <v>0</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O2" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P2">
         <v>75</v>
@@ -1498,15 +1498,15 @@
         <v>90</v>
       </c>
       <c r="V2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" ref="B3:B21" si="0">_xlfn.CONCAT(ROUND(F3,1),"%")</f>
@@ -1526,13 +1526,13 @@
         <v>5.2631578947368425</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O3" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P3">
         <v>75</v>
@@ -1547,15 +1547,15 @@
         <v>90</v>
       </c>
       <c r="V3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
@@ -1575,13 +1575,13 @@
         <v>10.526315789473685</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O4" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P4">
         <v>75</v>
@@ -1596,15 +1596,15 @@
         <v>90</v>
       </c>
       <c r="V4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
@@ -1624,13 +1624,13 @@
         <v>15.789473684210526</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O5" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P5">
         <v>75</v>
@@ -1645,15 +1645,15 @@
         <v>90</v>
       </c>
       <c r="V5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -1673,13 +1673,13 @@
         <v>21.05263157894737</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P6">
         <v>75</v>
@@ -1694,15 +1694,15 @@
         <v>90</v>
       </c>
       <c r="V6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
@@ -1722,13 +1722,13 @@
         <v>26.315789473684209</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O7" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P7">
         <v>75</v>
@@ -1743,15 +1743,15 @@
         <v>90</v>
       </c>
       <c r="V7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
@@ -1771,13 +1771,13 @@
         <v>31.578947368421051</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O8" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P8">
         <v>75</v>
@@ -1792,15 +1792,15 @@
         <v>90</v>
       </c>
       <c r="V8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
@@ -1820,13 +1820,13 @@
         <v>36.842105263157897</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O9" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P9">
         <v>75</v>
@@ -1841,15 +1841,15 @@
         <v>90</v>
       </c>
       <c r="V9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -1869,13 +1869,13 @@
         <v>42.10526315789474</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O10" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P10">
         <v>75</v>
@@ -1890,15 +1890,15 @@
         <v>90</v>
       </c>
       <c r="V10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -1918,13 +1918,13 @@
         <v>47.368421052631582</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O11" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P11">
         <v>75</v>
@@ -1939,15 +1939,15 @@
         <v>90</v>
       </c>
       <c r="V11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
@@ -1967,13 +1967,13 @@
         <v>52.631578947368418</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O12" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P12">
         <v>75</v>
@@ -1988,15 +1988,15 @@
         <v>90</v>
       </c>
       <c r="V12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
@@ -2016,13 +2016,13 @@
         <v>57.89473684210526</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O13" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P13">
         <v>75</v>
@@ -2037,15 +2037,15 @@
         <v>90</v>
       </c>
       <c r="V13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -2065,13 +2065,13 @@
         <v>63.157894736842103</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O14" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P14">
         <v>75</v>
@@ -2086,15 +2086,15 @@
         <v>90</v>
       </c>
       <c r="V14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -2114,13 +2114,13 @@
         <v>68.421052631578945</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O15" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P15">
         <v>75</v>
@@ -2135,15 +2135,15 @@
         <v>90</v>
       </c>
       <c r="V15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -2163,13 +2163,13 @@
         <v>73.684210526315795</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O16" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P16">
         <v>75</v>
@@ -2184,15 +2184,15 @@
         <v>90</v>
       </c>
       <c r="V16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
@@ -2212,13 +2212,13 @@
         <v>78.94736842105263</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L17" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O17" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P17">
         <v>75</v>
@@ -2233,15 +2233,15 @@
         <v>90</v>
       </c>
       <c r="V17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -2261,13 +2261,13 @@
         <v>84.21052631578948</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L18" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O18" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P18">
         <v>75</v>
@@ -2282,15 +2282,15 @@
         <v>90</v>
       </c>
       <c r="V18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
@@ -2310,13 +2310,13 @@
         <v>89.473684210526315</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L19" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O19" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P19">
         <v>75</v>
@@ -2331,15 +2331,15 @@
         <v>90</v>
       </c>
       <c r="V19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
@@ -2359,13 +2359,13 @@
         <v>94.736842105263165</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L20" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O20" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P20">
         <v>75</v>
@@ -2380,15 +2380,15 @@
         <v>90</v>
       </c>
       <c r="V20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
@@ -2408,13 +2408,13 @@
         <v>100</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L21" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O21" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P21">
         <v>75</v>
@@ -2429,10 +2429,10 @@
         <v>90</v>
       </c>
       <c r="V21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="W21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2448,7 +2448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -2518,16 +2518,16 @@
         <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" t="s">
         <v>86</v>
-      </c>
-      <c r="G2" t="s">
-        <v>87</v>
       </c>
       <c r="H2">
         <v>14</v>
@@ -2542,16 +2542,16 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" t="s">
         <v>83</v>
       </c>
-      <c r="N2" t="s">
-        <v>83</v>
-      </c>
-      <c r="O2" t="s">
-        <v>84</v>
-      </c>
       <c r="P2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2598,7 +2598,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>81</v>
@@ -2607,7 +2607,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2738,10 +2738,10 @@
         <v>20.5</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2755,10 +2755,10 @@
         <v>20.5</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>